<commit_message>
fix hide/show for title type parent
</commit_message>
<xml_diff>
--- a/storage/excel/SurveyDB_v1.xlsx
+++ b/storage/excel/SurveyDB_v1.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12885" firstSheet="2" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12885" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="ตัวเลือก" sheetId="7" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3698" uniqueCount="617">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3698" uniqueCount="615">
   <si>
     <t>id</t>
   </si>
@@ -1231,12 +1231,6 @@
   </si>
   <si>
     <t>264, 265</t>
-  </si>
-  <si>
-    <t>264, 266</t>
-  </si>
-  <si>
-    <t>264, 267</t>
   </si>
   <si>
     <t>68, 70, 71</t>
@@ -2276,8 +2270,8 @@
   <dimension ref="A1:B385"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A294" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B384" sqref="B384"/>
+      <pane ySplit="1" topLeftCell="A156" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D164" sqref="D164"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2355,7 +2349,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
@@ -2363,7 +2357,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
@@ -2371,7 +2365,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
@@ -2379,7 +2373,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -2387,7 +2381,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
@@ -2395,7 +2389,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
@@ -2403,7 +2397,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
@@ -2411,7 +2405,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
@@ -2419,7 +2413,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
@@ -2427,7 +2421,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
@@ -2435,7 +2429,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
@@ -2443,7 +2437,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
@@ -2451,7 +2445,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
@@ -2459,7 +2453,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
@@ -2467,7 +2461,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
@@ -2475,7 +2469,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
@@ -2483,7 +2477,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
@@ -2491,7 +2485,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
@@ -2499,7 +2493,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
@@ -2507,7 +2501,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
@@ -2515,7 +2509,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
@@ -2523,7 +2517,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
@@ -2531,7 +2525,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
@@ -2539,7 +2533,7 @@
         <v>31</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
@@ -2547,7 +2541,7 @@
         <v>32</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
@@ -2555,7 +2549,7 @@
         <v>33</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
@@ -2563,7 +2557,7 @@
         <v>34</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
@@ -2571,7 +2565,7 @@
         <v>35</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
@@ -2579,7 +2573,7 @@
         <v>36</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
@@ -2587,7 +2581,7 @@
         <v>37</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
@@ -2595,7 +2589,7 @@
         <v>38</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
@@ -2603,7 +2597,7 @@
         <v>39</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
@@ -2611,7 +2605,7 @@
         <v>40</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
@@ -2619,7 +2613,7 @@
         <v>41</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
@@ -2627,7 +2621,7 @@
         <v>42</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
@@ -2635,7 +2629,7 @@
         <v>43</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
@@ -2643,7 +2637,7 @@
         <v>44</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
@@ -2659,7 +2653,7 @@
         <v>46</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
@@ -2667,7 +2661,7 @@
         <v>47</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
@@ -2675,7 +2669,7 @@
         <v>48</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
@@ -2683,7 +2677,7 @@
         <v>49</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
@@ -2691,7 +2685,7 @@
         <v>50</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
@@ -2699,7 +2693,7 @@
         <v>51</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
@@ -2707,7 +2701,7 @@
         <v>52</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
@@ -2715,7 +2709,7 @@
         <v>53</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
@@ -2723,7 +2717,7 @@
         <v>54</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
@@ -2731,7 +2725,7 @@
         <v>55</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
@@ -2739,7 +2733,7 @@
         <v>56</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
@@ -2747,7 +2741,7 @@
         <v>57</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
@@ -2755,7 +2749,7 @@
         <v>58</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
@@ -2763,7 +2757,7 @@
         <v>59</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.2">
@@ -2771,7 +2765,7 @@
         <v>60</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
@@ -2779,7 +2773,7 @@
         <v>61</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.2">
@@ -2787,7 +2781,7 @@
         <v>62</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.2">
@@ -2795,7 +2789,7 @@
         <v>63</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.2">
@@ -2803,7 +2797,7 @@
         <v>64</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.2">
@@ -2811,7 +2805,7 @@
         <v>65</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.2">
@@ -2819,7 +2813,7 @@
         <v>66</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.2">
@@ -2827,7 +2821,7 @@
         <v>67</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.2">
@@ -4059,7 +4053,7 @@
         <v>221</v>
       </c>
       <c r="B222" s="1" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
     </row>
     <row r="223" spans="1:2" x14ac:dyDescent="0.2">
@@ -4067,7 +4061,7 @@
         <v>222</v>
       </c>
       <c r="B223" s="1" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.2">
@@ -4075,7 +4069,7 @@
         <v>223</v>
       </c>
       <c r="B224" s="1" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.2">
@@ -4083,7 +4077,7 @@
         <v>224</v>
       </c>
       <c r="B225" s="1" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.2">
@@ -4091,7 +4085,7 @@
         <v>225</v>
       </c>
       <c r="B226" s="1" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
     </row>
     <row r="227" spans="1:2" x14ac:dyDescent="0.2">
@@ -4099,7 +4093,7 @@
         <v>226</v>
       </c>
       <c r="B227" s="1" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
     </row>
     <row r="228" spans="1:2" x14ac:dyDescent="0.2">
@@ -4387,7 +4381,7 @@
         <v>262</v>
       </c>
       <c r="B263" s="6" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
     </row>
     <row r="264" spans="1:2" x14ac:dyDescent="0.2">
@@ -4619,7 +4613,7 @@
         <v>291</v>
       </c>
       <c r="B292" s="6" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
     </row>
     <row r="293" spans="1:2" x14ac:dyDescent="0.2">
@@ -4627,7 +4621,7 @@
         <v>292</v>
       </c>
       <c r="B293" s="6" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
     </row>
     <row r="294" spans="1:2" x14ac:dyDescent="0.2">
@@ -4635,7 +4629,7 @@
         <v>293</v>
       </c>
       <c r="B294" s="6" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
     </row>
     <row r="295" spans="1:2" x14ac:dyDescent="0.2">
@@ -4771,7 +4765,7 @@
         <v>310</v>
       </c>
       <c r="B311" s="6" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
     </row>
     <row r="312" spans="1:2" x14ac:dyDescent="0.2">
@@ -4779,7 +4773,7 @@
         <v>311</v>
       </c>
       <c r="B312" s="6" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
     </row>
     <row r="313" spans="1:2" x14ac:dyDescent="0.2">
@@ -4787,7 +4781,7 @@
         <v>312</v>
       </c>
       <c r="B313" s="6" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
     </row>
     <row r="314" spans="1:2" x14ac:dyDescent="0.2">
@@ -4795,7 +4789,7 @@
         <v>313</v>
       </c>
       <c r="B314" s="6" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="315" spans="1:2" x14ac:dyDescent="0.2">
@@ -4803,7 +4797,7 @@
         <v>314</v>
       </c>
       <c r="B315" s="6" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
     </row>
     <row r="316" spans="1:2" x14ac:dyDescent="0.2">
@@ -4811,7 +4805,7 @@
         <v>315</v>
       </c>
       <c r="B316" s="6" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
     </row>
     <row r="317" spans="1:2" x14ac:dyDescent="0.2">
@@ -4819,7 +4813,7 @@
         <v>316</v>
       </c>
       <c r="B317" s="6" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
     </row>
     <row r="318" spans="1:2" x14ac:dyDescent="0.2">
@@ -4827,7 +4821,7 @@
         <v>317</v>
       </c>
       <c r="B318" s="6" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
     </row>
     <row r="319" spans="1:2" x14ac:dyDescent="0.2">
@@ -4835,7 +4829,7 @@
         <v>318</v>
       </c>
       <c r="B319" s="6" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
     </row>
     <row r="320" spans="1:2" x14ac:dyDescent="0.2">
@@ -4843,7 +4837,7 @@
         <v>319</v>
       </c>
       <c r="B320" s="1" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
     </row>
     <row r="321" spans="1:2" x14ac:dyDescent="0.2">
@@ -4851,7 +4845,7 @@
         <v>320</v>
       </c>
       <c r="B321" s="1" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
     </row>
     <row r="322" spans="1:2" x14ac:dyDescent="0.2">
@@ -4859,7 +4853,7 @@
         <v>321</v>
       </c>
       <c r="B322" s="1" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
     </row>
     <row r="323" spans="1:2" x14ac:dyDescent="0.2">
@@ -4867,7 +4861,7 @@
         <v>322</v>
       </c>
       <c r="B323" s="1" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
     </row>
     <row r="324" spans="1:2" x14ac:dyDescent="0.2">
@@ -4875,7 +4869,7 @@
         <v>323</v>
       </c>
       <c r="B324" s="1" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
     </row>
     <row r="325" spans="1:2" x14ac:dyDescent="0.2">
@@ -4883,7 +4877,7 @@
         <v>324</v>
       </c>
       <c r="B325" s="1" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
     </row>
     <row r="326" spans="1:2" x14ac:dyDescent="0.2">
@@ -4891,7 +4885,7 @@
         <v>325</v>
       </c>
       <c r="B326" s="1" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
     </row>
     <row r="327" spans="1:2" x14ac:dyDescent="0.2">
@@ -4899,7 +4893,7 @@
         <v>326</v>
       </c>
       <c r="B327" s="1" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="328" spans="1:2" x14ac:dyDescent="0.2">
@@ -4907,7 +4901,7 @@
         <v>327</v>
       </c>
       <c r="B328" s="1" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
     </row>
     <row r="329" spans="1:2" x14ac:dyDescent="0.2">
@@ -4915,7 +4909,7 @@
         <v>328</v>
       </c>
       <c r="B329" s="1" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
     </row>
     <row r="330" spans="1:2" x14ac:dyDescent="0.2">
@@ -4923,7 +4917,7 @@
         <v>329</v>
       </c>
       <c r="B330" s="1" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
     </row>
     <row r="331" spans="1:2" x14ac:dyDescent="0.2">
@@ -4931,7 +4925,7 @@
         <v>330</v>
       </c>
       <c r="B331" s="1" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
     </row>
     <row r="332" spans="1:2" x14ac:dyDescent="0.2">
@@ -4939,7 +4933,7 @@
         <v>331</v>
       </c>
       <c r="B332" s="1" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
     </row>
     <row r="333" spans="1:2" x14ac:dyDescent="0.2">
@@ -4947,7 +4941,7 @@
         <v>332</v>
       </c>
       <c r="B333" s="1" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
     </row>
     <row r="334" spans="1:2" x14ac:dyDescent="0.2">
@@ -4955,7 +4949,7 @@
         <v>333</v>
       </c>
       <c r="B334" s="1" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
     </row>
     <row r="335" spans="1:2" x14ac:dyDescent="0.2">
@@ -4963,7 +4957,7 @@
         <v>334</v>
       </c>
       <c r="B335" s="1" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="336" spans="1:2" x14ac:dyDescent="0.2">
@@ -4971,7 +4965,7 @@
         <v>335</v>
       </c>
       <c r="B336" s="1" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
     </row>
     <row r="337" spans="1:2" x14ac:dyDescent="0.2">
@@ -4979,7 +4973,7 @@
         <v>336</v>
       </c>
       <c r="B337" s="1" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
     </row>
     <row r="338" spans="1:2" x14ac:dyDescent="0.2">
@@ -4987,7 +4981,7 @@
         <v>337</v>
       </c>
       <c r="B338" s="1" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
     </row>
     <row r="339" spans="1:2" x14ac:dyDescent="0.2">
@@ -4995,7 +4989,7 @@
         <v>338</v>
       </c>
       <c r="B339" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
     </row>
     <row r="340" spans="1:2" x14ac:dyDescent="0.2">
@@ -5003,7 +4997,7 @@
         <v>339</v>
       </c>
       <c r="B340" s="1" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
     </row>
     <row r="341" spans="1:2" x14ac:dyDescent="0.2">
@@ -5011,7 +5005,7 @@
         <v>340</v>
       </c>
       <c r="B341" s="1" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
     </row>
     <row r="342" spans="1:2" x14ac:dyDescent="0.2">
@@ -5019,7 +5013,7 @@
         <v>341</v>
       </c>
       <c r="B342" s="1" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
     </row>
     <row r="343" spans="1:2" x14ac:dyDescent="0.2">
@@ -5027,7 +5021,7 @@
         <v>342</v>
       </c>
       <c r="B343" s="1" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
     </row>
     <row r="344" spans="1:2" x14ac:dyDescent="0.2">
@@ -5035,7 +5029,7 @@
         <v>343</v>
       </c>
       <c r="B344" s="1" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
     </row>
     <row r="345" spans="1:2" x14ac:dyDescent="0.2">
@@ -5043,7 +5037,7 @@
         <v>344</v>
       </c>
       <c r="B345" s="1" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
     </row>
     <row r="346" spans="1:2" x14ac:dyDescent="0.2">
@@ -5051,7 +5045,7 @@
         <v>345</v>
       </c>
       <c r="B346" s="1" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
     </row>
     <row r="347" spans="1:2" x14ac:dyDescent="0.2">
@@ -5059,7 +5053,7 @@
         <v>346</v>
       </c>
       <c r="B347" s="1" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
     </row>
     <row r="348" spans="1:2" x14ac:dyDescent="0.2">
@@ -5067,7 +5061,7 @@
         <v>347</v>
       </c>
       <c r="B348" s="1" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
     </row>
     <row r="349" spans="1:2" x14ac:dyDescent="0.2">
@@ -5075,7 +5069,7 @@
         <v>348</v>
       </c>
       <c r="B349" s="1" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
     </row>
     <row r="350" spans="1:2" x14ac:dyDescent="0.2">
@@ -5083,7 +5077,7 @@
         <v>349</v>
       </c>
       <c r="B350" s="1" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
     </row>
     <row r="351" spans="1:2" x14ac:dyDescent="0.2">
@@ -5091,7 +5085,7 @@
         <v>350</v>
       </c>
       <c r="B351" s="1" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
     </row>
     <row r="352" spans="1:2" x14ac:dyDescent="0.2">
@@ -5099,7 +5093,7 @@
         <v>351</v>
       </c>
       <c r="B352" s="1" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
     </row>
     <row r="353" spans="1:2" x14ac:dyDescent="0.2">
@@ -5107,7 +5101,7 @@
         <v>352</v>
       </c>
       <c r="B353" s="1" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
     </row>
     <row r="354" spans="1:2" x14ac:dyDescent="0.2">
@@ -5115,7 +5109,7 @@
         <v>353</v>
       </c>
       <c r="B354" s="1" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
     </row>
     <row r="355" spans="1:2" x14ac:dyDescent="0.2">
@@ -5123,7 +5117,7 @@
         <v>354</v>
       </c>
       <c r="B355" s="1" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
     </row>
     <row r="356" spans="1:2" x14ac:dyDescent="0.2">
@@ -5131,7 +5125,7 @@
         <v>355</v>
       </c>
       <c r="B356" s="1" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
     </row>
     <row r="357" spans="1:2" x14ac:dyDescent="0.2">
@@ -5139,7 +5133,7 @@
         <v>356</v>
       </c>
       <c r="B357" s="1" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
     </row>
     <row r="358" spans="1:2" x14ac:dyDescent="0.2">
@@ -5147,7 +5141,7 @@
         <v>357</v>
       </c>
       <c r="B358" s="1" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
     </row>
     <row r="359" spans="1:2" x14ac:dyDescent="0.2">
@@ -5155,7 +5149,7 @@
         <v>358</v>
       </c>
       <c r="B359" s="1" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
     </row>
     <row r="360" spans="1:2" x14ac:dyDescent="0.2">
@@ -5163,7 +5157,7 @@
         <v>359</v>
       </c>
       <c r="B360" s="1" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
     </row>
     <row r="361" spans="1:2" x14ac:dyDescent="0.2">
@@ -5171,7 +5165,7 @@
         <v>360</v>
       </c>
       <c r="B361" s="1" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
     </row>
     <row r="362" spans="1:2" x14ac:dyDescent="0.2">
@@ -5179,7 +5173,7 @@
         <v>361</v>
       </c>
       <c r="B362" s="1" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
     </row>
     <row r="363" spans="1:2" x14ac:dyDescent="0.2">
@@ -5187,7 +5181,7 @@
         <v>362</v>
       </c>
       <c r="B363" s="1" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
     </row>
     <row r="364" spans="1:2" x14ac:dyDescent="0.2">
@@ -5195,7 +5189,7 @@
         <v>363</v>
       </c>
       <c r="B364" s="1" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
     </row>
     <row r="365" spans="1:2" x14ac:dyDescent="0.2">
@@ -5203,7 +5197,7 @@
         <v>364</v>
       </c>
       <c r="B365" s="1" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
     </row>
     <row r="366" spans="1:2" x14ac:dyDescent="0.2">
@@ -5211,7 +5205,7 @@
         <v>365</v>
       </c>
       <c r="B366" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
     </row>
     <row r="367" spans="1:2" x14ac:dyDescent="0.2">
@@ -5219,7 +5213,7 @@
         <v>366</v>
       </c>
       <c r="B367" s="1" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
     </row>
     <row r="368" spans="1:2" x14ac:dyDescent="0.2">
@@ -5227,7 +5221,7 @@
         <v>367</v>
       </c>
       <c r="B368" s="1" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
     </row>
     <row r="369" spans="1:2" x14ac:dyDescent="0.2">
@@ -5235,7 +5229,7 @@
         <v>368</v>
       </c>
       <c r="B369" s="1" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
     </row>
     <row r="370" spans="1:2" x14ac:dyDescent="0.2">
@@ -5243,7 +5237,7 @@
         <v>369</v>
       </c>
       <c r="B370" s="1" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
     </row>
     <row r="371" spans="1:2" x14ac:dyDescent="0.2">
@@ -5251,7 +5245,7 @@
         <v>370</v>
       </c>
       <c r="B371" s="1" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
     </row>
     <row r="372" spans="1:2" x14ac:dyDescent="0.2">
@@ -5259,7 +5253,7 @@
         <v>371</v>
       </c>
       <c r="B372" s="1" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
     </row>
     <row r="373" spans="1:2" x14ac:dyDescent="0.2">
@@ -5267,7 +5261,7 @@
         <v>372</v>
       </c>
       <c r="B373" s="1" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
     </row>
     <row r="374" spans="1:2" x14ac:dyDescent="0.2">
@@ -5275,7 +5269,7 @@
         <v>373</v>
       </c>
       <c r="B374" s="1" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
     </row>
     <row r="375" spans="1:2" x14ac:dyDescent="0.2">
@@ -5283,7 +5277,7 @@
         <v>374</v>
       </c>
       <c r="B375" s="1" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
     </row>
     <row r="376" spans="1:2" x14ac:dyDescent="0.2">
@@ -5291,7 +5285,7 @@
         <v>375</v>
       </c>
       <c r="B376" s="1" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
     </row>
     <row r="377" spans="1:2" x14ac:dyDescent="0.2">
@@ -5299,7 +5293,7 @@
         <v>376</v>
       </c>
       <c r="B377" s="1" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
     </row>
     <row r="378" spans="1:2" x14ac:dyDescent="0.2">
@@ -5307,7 +5301,7 @@
         <v>377</v>
       </c>
       <c r="B378" s="1" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
     </row>
     <row r="379" spans="1:2" x14ac:dyDescent="0.2">
@@ -5315,7 +5309,7 @@
         <v>378</v>
       </c>
       <c r="B379" s="1" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
     </row>
     <row r="380" spans="1:2" x14ac:dyDescent="0.2">
@@ -5323,7 +5317,7 @@
         <v>379</v>
       </c>
       <c r="B380" s="1" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
     </row>
     <row r="381" spans="1:2" x14ac:dyDescent="0.2">
@@ -5331,7 +5325,7 @@
         <v>380</v>
       </c>
       <c r="B381" s="1" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
     </row>
     <row r="382" spans="1:2" x14ac:dyDescent="0.2">
@@ -5339,7 +5333,7 @@
         <v>381</v>
       </c>
       <c r="B382" s="1" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
     </row>
     <row r="383" spans="1:2" x14ac:dyDescent="0.2">
@@ -5347,7 +5341,7 @@
         <v>382</v>
       </c>
       <c r="B383" s="1" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
     </row>
     <row r="384" spans="1:2" x14ac:dyDescent="0.2">
@@ -5355,7 +5349,7 @@
         <v>383</v>
       </c>
       <c r="B384" s="1" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
     </row>
     <row r="385" spans="1:2" x14ac:dyDescent="0.2">
@@ -5363,7 +5357,7 @@
         <v>384</v>
       </c>
       <c r="B385" s="1" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
     </row>
   </sheetData>
@@ -5376,8 +5370,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -5445,7 +5439,7 @@
         <v>7</v>
       </c>
       <c r="H2" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
@@ -5471,7 +5465,7 @@
         <v>7</v>
       </c>
       <c r="H3" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
@@ -5485,7 +5479,7 @@
         <v>2</v>
       </c>
       <c r="D4" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="E4" t="s">
         <v>395</v>
@@ -5497,7 +5491,7 @@
         <v>7</v>
       </c>
       <c r="H4" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
@@ -5511,7 +5505,7 @@
         <v>3</v>
       </c>
       <c r="D5" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="E5" t="s">
         <v>395</v>
@@ -5523,7 +5517,7 @@
         <v>11</v>
       </c>
       <c r="H5" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
@@ -5549,7 +5543,7 @@
         <v>7</v>
       </c>
       <c r="H6" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
@@ -5575,7 +5569,7 @@
         <v>7</v>
       </c>
       <c r="H7" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
@@ -5589,7 +5583,7 @@
         <v>2</v>
       </c>
       <c r="D8" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="E8" t="s">
         <v>396</v>
@@ -5601,7 +5595,7 @@
         <v>7</v>
       </c>
       <c r="H8" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
@@ -5615,7 +5609,7 @@
         <v>3</v>
       </c>
       <c r="D9" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="E9" t="s">
         <v>396</v>
@@ -5627,7 +5621,7 @@
         <v>11</v>
       </c>
       <c r="H9" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
@@ -5653,7 +5647,7 @@
         <v>7</v>
       </c>
       <c r="H10" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
@@ -5679,7 +5673,7 @@
         <v>7</v>
       </c>
       <c r="H11" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
@@ -5693,7 +5687,7 @@
         <v>2</v>
       </c>
       <c r="D12" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="E12" t="s">
         <v>397</v>
@@ -5705,7 +5699,7 @@
         <v>7</v>
       </c>
       <c r="H12" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
@@ -5719,7 +5713,7 @@
         <v>3</v>
       </c>
       <c r="D13" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="E13" t="s">
         <v>397</v>
@@ -5731,7 +5725,7 @@
         <v>11</v>
       </c>
       <c r="H13" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
     </row>
   </sheetData>
@@ -5743,7 +5737,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C78"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -6622,8 +6616,8 @@
   <dimension ref="A1:M58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F8" sqref="F8"/>
+      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D59" sqref="D59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -6632,7 +6626,7 @@
     <col min="2" max="2" width="16.75" customWidth="1"/>
     <col min="3" max="3" width="11.875" customWidth="1"/>
     <col min="4" max="4" width="32.875" customWidth="1"/>
-    <col min="5" max="5" width="21.375" customWidth="1"/>
+    <col min="5" max="5" width="40" customWidth="1"/>
     <col min="6" max="6" width="19.875" customWidth="1"/>
     <col min="7" max="7" width="15" customWidth="1"/>
     <col min="8" max="8" width="38.625" customWidth="1"/>
@@ -6683,7 +6677,7 @@
         <v>172</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="F2" s="9" t="s">
         <v>172</v>
@@ -6692,7 +6686,7 @@
         <v>35</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="I2" s="9"/>
       <c r="J2" s="9"/>
@@ -6711,7 +6705,7 @@
         <v>172</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="F3" t="s">
         <v>172</v>
@@ -6742,7 +6736,7 @@
         <v>172</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="F4" t="s">
         <v>172</v>
@@ -6751,7 +6745,7 @@
         <v>35</v>
       </c>
       <c r="H4" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="I4" t="s">
         <v>172</v>
@@ -6773,7 +6767,7 @@
         <v>172</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="F5" t="s">
         <v>172</v>
@@ -6804,7 +6798,7 @@
         <v>172</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="F6" t="s">
         <v>172</v>
@@ -6835,7 +6829,7 @@
         <v>172</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="F7" t="s">
         <v>172</v>
@@ -6866,7 +6860,7 @@
         <v>172</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="F8" t="s">
         <v>172</v>
@@ -6897,7 +6891,7 @@
         <v>172</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="F9" t="s">
         <v>172</v>
@@ -6928,7 +6922,7 @@
         <v>172</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="F10" t="s">
         <v>172</v>
@@ -6937,7 +6931,7 @@
         <v>7</v>
       </c>
       <c r="H10" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="I10" t="s">
         <v>172</v>
@@ -6959,7 +6953,7 @@
         <v>2</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="F11" t="s">
         <v>172</v>
@@ -6990,7 +6984,7 @@
         <v>3</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="F12" t="s">
         <v>172</v>
@@ -7019,7 +7013,7 @@
         <v>172</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="F13" t="s">
         <v>172</v>
@@ -7028,7 +7022,7 @@
         <v>7</v>
       </c>
       <c r="H13" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="I13" t="s">
         <v>172</v>
@@ -7048,7 +7042,7 @@
         <v>4</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="F14" t="s">
         <v>172</v>
@@ -7077,7 +7071,7 @@
         <v>5</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="F15" t="s">
         <v>172</v>
@@ -7106,7 +7100,7 @@
         <v>172</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="F16" t="s">
         <v>172</v>
@@ -7115,7 +7109,7 @@
         <v>7</v>
       </c>
       <c r="H16" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="I16" t="s">
         <v>172</v>
@@ -7135,7 +7129,7 @@
         <v>6</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="F17" s="8" t="s">
         <v>172</v>
@@ -7144,7 +7138,7 @@
         <v>7</v>
       </c>
       <c r="H17" s="8" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="I17" s="8"/>
     </row>
@@ -7162,7 +7156,7 @@
         <v>7</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="F18" s="8" t="s">
         <v>172</v>
@@ -7171,7 +7165,7 @@
         <v>7</v>
       </c>
       <c r="H18" s="8" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="I18" s="8"/>
     </row>
@@ -7189,7 +7183,7 @@
         <v>172</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="F19" t="s">
         <v>172</v>
@@ -7218,7 +7212,7 @@
         <v>172</v>
       </c>
       <c r="E20" s="9" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="F20" t="s">
         <v>172</v>
@@ -7247,7 +7241,7 @@
         <v>172</v>
       </c>
       <c r="E21" s="9" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="F21" t="s">
         <v>172</v>
@@ -7276,7 +7270,7 @@
         <v>172</v>
       </c>
       <c r="E22" s="9" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="F22" t="s">
         <v>172</v>
@@ -7305,7 +7299,7 @@
         <v>172</v>
       </c>
       <c r="E23" s="9" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="F23" t="s">
         <v>172</v>
@@ -7334,7 +7328,7 @@
         <v>172</v>
       </c>
       <c r="E24" s="9" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="F24" t="s">
         <v>172</v>
@@ -7363,7 +7357,7 @@
         <v>172</v>
       </c>
       <c r="E25" s="9" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="F25" t="s">
         <v>172</v>
@@ -7392,7 +7386,7 @@
         <v>172</v>
       </c>
       <c r="E26" s="9" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="F26" t="s">
         <v>172</v>
@@ -7421,7 +7415,7 @@
         <v>172</v>
       </c>
       <c r="E27" s="9" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="F27" t="s">
         <v>172</v>
@@ -7450,7 +7444,7 @@
         <v>172</v>
       </c>
       <c r="E28" s="9" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="F28" t="s">
         <v>172</v>
@@ -7479,7 +7473,7 @@
         <v>172</v>
       </c>
       <c r="E29" s="9" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="F29" t="s">
         <v>172</v>
@@ -7508,7 +7502,7 @@
         <v>172</v>
       </c>
       <c r="E30" s="9" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="F30" t="s">
         <v>172</v>
@@ -7537,7 +7531,7 @@
         <v>172</v>
       </c>
       <c r="E31" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="F31" t="s">
         <v>172</v>
@@ -7546,7 +7540,7 @@
         <v>7</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="I31" t="s">
         <v>172</v>
@@ -7560,13 +7554,13 @@
         <v>172</v>
       </c>
       <c r="C32">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D32" t="s">
         <v>172</v>
       </c>
       <c r="E32" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="F32" t="s">
         <v>172</v>
@@ -7575,7 +7569,7 @@
         <v>7</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="I32" t="s">
         <v>172</v>
@@ -7595,7 +7589,7 @@
         <v>172</v>
       </c>
       <c r="E33" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="F33" s="7" t="s">
         <v>172</v>
@@ -7604,7 +7598,7 @@
         <v>7</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="I33" s="7" t="s">
         <v>172</v>
@@ -7624,7 +7618,7 @@
         <v>172</v>
       </c>
       <c r="E34" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="F34" t="s">
         <v>172</v>
@@ -7633,7 +7627,7 @@
         <v>7</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="I34" t="s">
         <v>172</v>
@@ -7653,7 +7647,7 @@
         <v>172</v>
       </c>
       <c r="E35" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="F35" t="s">
         <v>172</v>
@@ -7662,7 +7656,7 @@
         <v>11</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="I35" t="s">
         <v>172</v>
@@ -7682,7 +7676,7 @@
         <v>172</v>
       </c>
       <c r="E36" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="F36" t="s">
         <v>172</v>
@@ -7691,7 +7685,7 @@
         <v>7</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="I36" t="s">
         <v>172</v>
@@ -7711,7 +7705,7 @@
         <v>172</v>
       </c>
       <c r="E37" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="F37" t="s">
         <v>172</v>
@@ -7720,7 +7714,7 @@
         <v>7</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="I37" t="s">
         <v>172</v>
@@ -7740,7 +7734,7 @@
         <v>172</v>
       </c>
       <c r="E38" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="F38" t="s">
         <v>172</v>
@@ -7749,7 +7743,7 @@
         <v>35</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="I38" t="s">
         <v>172</v>
@@ -7769,7 +7763,7 @@
         <v>172</v>
       </c>
       <c r="E39" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="F39" t="s">
         <v>172</v>
@@ -7798,7 +7792,7 @@
         <v>172</v>
       </c>
       <c r="E40" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="F40" t="s">
         <v>172</v>
@@ -7807,7 +7801,7 @@
         <v>35</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="I40" t="s">
         <v>172</v>
@@ -7827,7 +7821,7 @@
         <v>172</v>
       </c>
       <c r="E41" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="F41" t="s">
         <v>172</v>
@@ -7856,7 +7850,7 @@
         <v>172</v>
       </c>
       <c r="E42" s="8" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="F42" s="8" t="s">
         <v>172</v>
@@ -7865,7 +7859,7 @@
         <v>11</v>
       </c>
       <c r="H42" s="9" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="I42" s="8"/>
     </row>
@@ -7883,7 +7877,7 @@
         <v>172</v>
       </c>
       <c r="E43" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="F43" t="s">
         <v>172</v>
@@ -7912,7 +7906,7 @@
         <v>172</v>
       </c>
       <c r="E44" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="F44" t="s">
         <v>172</v>
@@ -7941,7 +7935,7 @@
         <v>172</v>
       </c>
       <c r="E45" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="F45" t="s">
         <v>172</v>
@@ -7970,7 +7964,7 @@
         <v>172</v>
       </c>
       <c r="E46" s="8" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="F46" s="8" t="s">
         <v>172</v>
@@ -7979,7 +7973,7 @@
         <v>11</v>
       </c>
       <c r="H46" s="9" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="I46" s="8"/>
     </row>
@@ -7997,7 +7991,7 @@
         <v>172</v>
       </c>
       <c r="E47" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="F47" t="s">
         <v>172</v>
@@ -8026,7 +8020,7 @@
         <v>172</v>
       </c>
       <c r="E48" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="F48" t="s">
         <v>172</v>
@@ -8035,7 +8029,7 @@
         <v>7</v>
       </c>
       <c r="H48" s="2" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="I48" t="s">
         <v>172</v>
@@ -8055,7 +8049,7 @@
         <v>172</v>
       </c>
       <c r="E49" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="F49" t="s">
         <v>172</v>
@@ -8064,7 +8058,7 @@
         <v>7</v>
       </c>
       <c r="H49" s="2" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="I49" t="s">
         <v>172</v>
@@ -8084,7 +8078,7 @@
         <v>172</v>
       </c>
       <c r="E50" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="F50" t="s">
         <v>172</v>
@@ -8093,7 +8087,7 @@
         <v>7</v>
       </c>
       <c r="H50" s="2" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="I50" t="s">
         <v>172</v>
@@ -8113,7 +8107,7 @@
         <v>172</v>
       </c>
       <c r="E51" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="F51" t="s">
         <v>172</v>
@@ -8122,7 +8116,7 @@
         <v>35</v>
       </c>
       <c r="H51" s="2" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="I51" t="s">
         <v>172</v>
@@ -8142,7 +8136,7 @@
         <v>172</v>
       </c>
       <c r="E52" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="F52" t="s">
         <v>172</v>
@@ -8171,7 +8165,7 @@
         <v>172</v>
       </c>
       <c r="E53" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="F53" t="s">
         <v>172</v>
@@ -8200,7 +8194,7 @@
         <v>172</v>
       </c>
       <c r="E54" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="F54" t="s">
         <v>172</v>
@@ -8209,7 +8203,7 @@
         <v>35</v>
       </c>
       <c r="H54" s="2" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="I54" t="s">
         <v>172</v>
@@ -8229,7 +8223,7 @@
         <v>172</v>
       </c>
       <c r="E55" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="F55" t="s">
         <v>172</v>
@@ -8258,7 +8252,7 @@
         <v>172</v>
       </c>
       <c r="E56" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="F56" t="s">
         <v>172</v>
@@ -8287,7 +8281,7 @@
         <v>172</v>
       </c>
       <c r="E57" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="F57" t="s">
         <v>172</v>
@@ -8296,7 +8290,7 @@
         <v>7</v>
       </c>
       <c r="H57" s="2" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="I57" t="s">
         <v>172</v>
@@ -8316,7 +8310,7 @@
         <v>66</v>
       </c>
       <c r="E58" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="F58" t="s">
         <v>172</v>
@@ -9429,16 +9423,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I418"/>
   <sheetViews>
-    <sheetView topLeftCell="A147" workbookViewId="0">
-      <selection activeCell="C190" sqref="C190"/>
+    <sheetView topLeftCell="A87" workbookViewId="0">
+      <selection activeCell="G109" sqref="G109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5.125" customWidth="1"/>
-    <col min="2" max="2" width="11.875" customWidth="1"/>
-    <col min="3" max="3" width="5.875" customWidth="1"/>
-    <col min="4" max="4" width="14.25" customWidth="1"/>
+    <col min="2" max="2" width="12" customWidth="1"/>
+    <col min="3" max="3" width="6" customWidth="1"/>
+    <col min="4" max="4" width="14.125" customWidth="1"/>
     <col min="5" max="5" width="33.625" customWidth="1"/>
     <col min="6" max="6" width="28.25" customWidth="1"/>
     <col min="7" max="7" width="17" customWidth="1"/>
@@ -9498,7 +9492,7 @@
         <v>11</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="I2" s="9" t="s">
         <v>172</v>
@@ -9573,7 +9567,7 @@
         <v>2</v>
       </c>
       <c r="D5" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="E5" t="s">
         <v>381</v>
@@ -9602,7 +9596,7 @@
         <v>3</v>
       </c>
       <c r="D6" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="E6" t="s">
         <v>381</v>
@@ -9631,7 +9625,7 @@
         <v>4</v>
       </c>
       <c r="D7" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="E7" t="s">
         <v>381</v>
@@ -9660,7 +9654,7 @@
         <v>5</v>
       </c>
       <c r="D8" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="E8" t="s">
         <v>381</v>
@@ -9863,7 +9857,7 @@
         <v>2</v>
       </c>
       <c r="D15" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="E15" t="s">
         <v>381</v>
@@ -9892,7 +9886,7 @@
         <v>3</v>
       </c>
       <c r="D16" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="E16" t="s">
         <v>381</v>
@@ -9921,7 +9915,7 @@
         <v>4</v>
       </c>
       <c r="D17" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="E17" t="s">
         <v>381</v>
@@ -9950,7 +9944,7 @@
         <v>5</v>
       </c>
       <c r="D18" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="E18" t="s">
         <v>381</v>
@@ -10107,7 +10101,7 @@
         <v>11</v>
       </c>
       <c r="H23" s="8" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="I23" s="9" t="s">
         <v>172</v>
@@ -10356,7 +10350,7 @@
         <v>2</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="E32" s="8" t="s">
         <v>382</v>
@@ -12135,7 +12129,7 @@
         <v>11</v>
       </c>
       <c r="H93" s="8" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="I93" s="8" t="s">
         <v>172</v>
@@ -12335,7 +12329,7 @@
         <v>279</v>
       </c>
       <c r="G100" s="4" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="H100" s="2" t="s">
         <v>281</v>
@@ -12483,7 +12477,7 @@
         <v>11</v>
       </c>
       <c r="H105" s="8" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="I105" s="8" t="s">
         <v>172</v>
@@ -13237,7 +13231,7 @@
         <v>11</v>
       </c>
       <c r="H131" s="8" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="I131" s="8" t="s">
         <v>172</v>
@@ -14655,7 +14649,7 @@
         <v>34</v>
       </c>
       <c r="G180" s="8" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="H180" s="9" t="s">
         <v>286</v>
@@ -14829,7 +14823,7 @@
         <v>34</v>
       </c>
       <c r="G186" s="8" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="H186" s="9" t="s">
         <v>286</v>
@@ -15180,7 +15174,7 @@
         <v>29</v>
       </c>
       <c r="H198" s="2" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="I198" t="s">
         <v>378</v>
@@ -15209,7 +15203,7 @@
         <v>29</v>
       </c>
       <c r="H199" s="2" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="I199" t="s">
         <v>379</v>
@@ -15325,7 +15319,7 @@
         <v>29</v>
       </c>
       <c r="H203" s="2" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="I203" t="s">
         <v>378</v>
@@ -15354,7 +15348,7 @@
         <v>29</v>
       </c>
       <c r="H204" s="2" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="I204" t="s">
         <v>379</v>
@@ -15412,7 +15406,7 @@
         <v>11</v>
       </c>
       <c r="H206" s="8" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="I206" s="8" t="s">
         <v>172</v>
@@ -18950,7 +18944,7 @@
         <v>11</v>
       </c>
       <c r="H328" s="8" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="I328" s="8" t="s">
         <v>172</v>
@@ -19124,7 +19118,7 @@
         <v>11</v>
       </c>
       <c r="H334" s="8" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="I334" s="8" t="s">
         <v>172</v>
@@ -19443,7 +19437,7 @@
         <v>11</v>
       </c>
       <c r="H345" s="8" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="I345" s="8" t="s">
         <v>172</v>
@@ -19704,7 +19698,7 @@
         <v>11</v>
       </c>
       <c r="H354" s="8" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="I354" s="8" t="s">
         <v>172</v>
@@ -19878,7 +19872,7 @@
         <v>11</v>
       </c>
       <c r="H360" s="8" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="I360" s="8" t="s">
         <v>172</v>
@@ -19907,7 +19901,7 @@
         <v>11</v>
       </c>
       <c r="H361" s="2" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="I361" t="s">
         <v>172</v>
@@ -20168,7 +20162,7 @@
         <v>11</v>
       </c>
       <c r="H370" s="2" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="I370" t="s">
         <v>172</v>
@@ -20429,7 +20423,7 @@
         <v>11</v>
       </c>
       <c r="H379" s="2" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="I379" t="s">
         <v>172</v>
@@ -20690,7 +20684,7 @@
         <v>11</v>
       </c>
       <c r="H388" s="8" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="I388" s="8" t="s">
         <v>172</v>
@@ -21574,10 +21568,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C392"/>
+  <dimension ref="A1:C396"/>
   <sheetViews>
-    <sheetView topLeftCell="A267" workbookViewId="0">
-      <selection activeCell="D392" sqref="D392"/>
+    <sheetView topLeftCell="A308" workbookViewId="0">
+      <selection activeCell="E337" sqref="E337"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -25142,10 +25136,10 @@
     </row>
     <row r="324" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A324">
-        <v>1007</v>
+        <v>1006</v>
       </c>
       <c r="B324">
-        <v>120</v>
+        <v>81</v>
       </c>
       <c r="C324">
         <v>1</v>
@@ -25153,10 +25147,10 @@
     </row>
     <row r="325" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A325">
-        <v>1007</v>
-      </c>
-      <c r="B325" s="1">
-        <v>121</v>
+        <v>1006</v>
+      </c>
+      <c r="B325">
+        <v>82</v>
       </c>
       <c r="C325">
         <v>2</v>
@@ -25164,7 +25158,7 @@
     </row>
     <row r="326" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A326">
-        <v>1008</v>
+        <v>1007</v>
       </c>
       <c r="B326">
         <v>120</v>
@@ -25175,7 +25169,7 @@
     </row>
     <row r="327" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A327">
-        <v>1008</v>
+        <v>1007</v>
       </c>
       <c r="B327" s="1">
         <v>121</v>
@@ -25186,7 +25180,7 @@
     </row>
     <row r="328" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A328">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="B328">
         <v>120</v>
@@ -25197,7 +25191,7 @@
     </row>
     <row r="329" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A329">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="B329" s="1">
         <v>121</v>
@@ -25208,10 +25202,10 @@
     </row>
     <row r="330" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A330">
-        <v>1010</v>
-      </c>
-      <c r="B330" s="1">
-        <v>130</v>
+        <v>1009</v>
+      </c>
+      <c r="B330">
+        <v>120</v>
       </c>
       <c r="C330">
         <v>1</v>
@@ -25219,10 +25213,10 @@
     </row>
     <row r="331" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A331">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="B331" s="1">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="C331">
         <v>2</v>
@@ -25230,10 +25224,10 @@
     </row>
     <row r="332" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A332">
-        <v>1011</v>
-      </c>
-      <c r="B332">
-        <v>78</v>
+        <v>1010</v>
+      </c>
+      <c r="B332" s="1">
+        <v>130</v>
       </c>
       <c r="C332">
         <v>1</v>
@@ -25241,10 +25235,10 @@
     </row>
     <row r="333" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A333">
-        <v>1011</v>
+        <v>1010</v>
       </c>
       <c r="B333" s="1">
-        <v>79</v>
+        <v>131</v>
       </c>
       <c r="C333">
         <v>2</v>
@@ -25252,10 +25246,10 @@
     </row>
     <row r="334" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A334">
-        <v>1018</v>
-      </c>
-      <c r="B334" s="1">
-        <v>97</v>
+        <v>1011</v>
+      </c>
+      <c r="B334">
+        <v>78</v>
       </c>
       <c r="C334">
         <v>1</v>
@@ -25263,54 +25257,54 @@
     </row>
     <row r="335" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A335">
-        <v>1022</v>
-      </c>
-      <c r="B335">
-        <v>130</v>
+        <v>1011</v>
+      </c>
+      <c r="B335" s="1">
+        <v>79</v>
       </c>
       <c r="C335">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="336" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A336">
-        <v>1022</v>
+        <v>1017</v>
       </c>
       <c r="B336" s="1">
-        <v>131</v>
+        <v>81</v>
       </c>
       <c r="C336">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="337" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A337">
-        <v>1023</v>
-      </c>
-      <c r="B337" s="1">
-        <v>329</v>
+        <v>1017</v>
+      </c>
+      <c r="B337">
+        <v>82</v>
       </c>
       <c r="C337">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="338" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A338">
-        <v>1023</v>
+        <v>1018</v>
       </c>
       <c r="B338" s="1">
-        <v>330</v>
+        <v>97</v>
       </c>
       <c r="C338">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="339" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A339">
-        <v>1024</v>
-      </c>
-      <c r="B339" s="1">
-        <v>331</v>
+        <v>1022</v>
+      </c>
+      <c r="B339">
+        <v>130</v>
       </c>
       <c r="C339">
         <v>1</v>
@@ -25318,10 +25312,10 @@
     </row>
     <row r="340" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A340">
-        <v>1024</v>
+        <v>1022</v>
       </c>
       <c r="B340" s="1">
-        <v>332</v>
+        <v>131</v>
       </c>
       <c r="C340">
         <v>2</v>
@@ -25329,24 +25323,24 @@
     </row>
     <row r="341" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A341">
-        <v>1024</v>
+        <v>1023</v>
       </c>
       <c r="B341" s="1">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="C341">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="342" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A342">
-        <v>1024</v>
+        <v>1023</v>
       </c>
       <c r="B342" s="1">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="C342">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="343" spans="1:3" x14ac:dyDescent="0.2">
@@ -25354,10 +25348,10 @@
         <v>1024</v>
       </c>
       <c r="B343" s="1">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="C343">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="344" spans="1:3" x14ac:dyDescent="0.2">
@@ -25365,10 +25359,10 @@
         <v>1024</v>
       </c>
       <c r="B344" s="1">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="C344">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="345" spans="1:3" x14ac:dyDescent="0.2">
@@ -25376,10 +25370,10 @@
         <v>1024</v>
       </c>
       <c r="B345" s="1">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="C345">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="346" spans="1:3" x14ac:dyDescent="0.2">
@@ -25387,10 +25381,10 @@
         <v>1024</v>
       </c>
       <c r="B346" s="1">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="C346">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="347" spans="1:3" x14ac:dyDescent="0.2">
@@ -25398,10 +25392,10 @@
         <v>1024</v>
       </c>
       <c r="B347" s="1">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="C347">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="348" spans="1:3" x14ac:dyDescent="0.2">
@@ -25409,65 +25403,65 @@
         <v>1024</v>
       </c>
       <c r="B348" s="1">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="C348">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="349" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A349">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="B349" s="1">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="C349">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="350" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A350">
-        <v>1026</v>
+        <v>1024</v>
       </c>
       <c r="B350" s="1">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="C350">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="351" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A351">
-        <v>1026</v>
+        <v>1024</v>
       </c>
       <c r="B351" s="1">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="C351">
-        <v>2</v>
+        <v>9</v>
       </c>
     </row>
     <row r="352" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A352">
-        <v>1026</v>
+        <v>1024</v>
       </c>
       <c r="B352" s="1">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="C352">
-        <v>3</v>
+        <v>10</v>
       </c>
     </row>
     <row r="353" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A353">
-        <v>1026</v>
+        <v>1025</v>
       </c>
       <c r="B353" s="1">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="C353">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="354" spans="1:3" x14ac:dyDescent="0.2">
@@ -25475,54 +25469,54 @@
         <v>1026</v>
       </c>
       <c r="B354" s="1">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="C354">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="355" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A355">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="B355" s="1">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="C355">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="356" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A356">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="B356" s="1">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="C356">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="357" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A357">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="B357" s="1">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="C357">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="358" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A358">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="B358" s="1">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="C358">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="359" spans="1:3" x14ac:dyDescent="0.2">
@@ -25530,10 +25524,10 @@
         <v>1027</v>
       </c>
       <c r="B359" s="1">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="C359">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="360" spans="1:3" x14ac:dyDescent="0.2">
@@ -25541,10 +25535,10 @@
         <v>1027</v>
       </c>
       <c r="B360" s="1">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="C360">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="361" spans="1:3" x14ac:dyDescent="0.2">
@@ -25552,10 +25546,10 @@
         <v>1027</v>
       </c>
       <c r="B361" s="1">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="C361">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="362" spans="1:3" x14ac:dyDescent="0.2">
@@ -25563,10 +25557,10 @@
         <v>1027</v>
       </c>
       <c r="B362" s="1">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="C362">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="363" spans="1:3" x14ac:dyDescent="0.2">
@@ -25574,54 +25568,54 @@
         <v>1027</v>
       </c>
       <c r="B363" s="1">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="C363">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="364" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A364">
-        <v>1028</v>
+        <v>1027</v>
       </c>
       <c r="B364" s="1">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="C364">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="365" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A365">
-        <v>1028</v>
+        <v>1027</v>
       </c>
       <c r="B365" s="1">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="C365">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="366" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A366">
-        <v>1028</v>
+        <v>1027</v>
       </c>
       <c r="B366" s="1">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="C366">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="367" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A367">
-        <v>1028</v>
+        <v>1027</v>
       </c>
       <c r="B367" s="1">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="C367">
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="368" spans="1:3" x14ac:dyDescent="0.2">
@@ -25629,10 +25623,10 @@
         <v>1028</v>
       </c>
       <c r="B368" s="1">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="C368">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="369" spans="1:3" x14ac:dyDescent="0.2">
@@ -25640,10 +25634,10 @@
         <v>1028</v>
       </c>
       <c r="B369" s="1">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="C369">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="370" spans="1:3" x14ac:dyDescent="0.2">
@@ -25651,10 +25645,10 @@
         <v>1028</v>
       </c>
       <c r="B370" s="1">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="C370">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="371" spans="1:3" x14ac:dyDescent="0.2">
@@ -25662,10 +25656,10 @@
         <v>1028</v>
       </c>
       <c r="B371" s="1">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="C371">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="372" spans="1:3" x14ac:dyDescent="0.2">
@@ -25673,10 +25667,10 @@
         <v>1028</v>
       </c>
       <c r="B372" s="1">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="C372">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="373" spans="1:3" x14ac:dyDescent="0.2">
@@ -25684,10 +25678,10 @@
         <v>1028</v>
       </c>
       <c r="B373" s="1">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="C373">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="374" spans="1:3" x14ac:dyDescent="0.2">
@@ -25695,10 +25689,10 @@
         <v>1028</v>
       </c>
       <c r="B374" s="1">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="C374">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="375" spans="1:3" x14ac:dyDescent="0.2">
@@ -25706,10 +25700,10 @@
         <v>1028</v>
       </c>
       <c r="B375" s="1">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="C375">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="376" spans="1:3" x14ac:dyDescent="0.2">
@@ -25717,10 +25711,10 @@
         <v>1028</v>
       </c>
       <c r="B376" s="1">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="C376">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="377" spans="1:3" x14ac:dyDescent="0.2">
@@ -25728,73 +25722,73 @@
         <v>1028</v>
       </c>
       <c r="B377" s="1">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="C377">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="378" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A378">
-        <v>1029</v>
+        <v>1028</v>
       </c>
       <c r="B378" s="1">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="C378">
-        <v>1</v>
+        <v>11</v>
       </c>
     </row>
     <row r="379" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A379">
-        <v>1030</v>
+        <v>1028</v>
       </c>
       <c r="B379" s="1">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="C379">
-        <v>1</v>
+        <v>12</v>
       </c>
     </row>
     <row r="380" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A380">
-        <v>1030</v>
+        <v>1028</v>
       </c>
       <c r="B380" s="1">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="C380">
-        <v>2</v>
+        <v>13</v>
       </c>
     </row>
     <row r="381" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A381">
-        <v>1031</v>
+        <v>1028</v>
       </c>
       <c r="B381" s="1">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="C381">
-        <v>1</v>
+        <v>14</v>
       </c>
     </row>
     <row r="382" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A382">
-        <v>1031</v>
+        <v>1029</v>
       </c>
       <c r="B382" s="1">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="C382">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="383" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A383">
-        <v>1032</v>
+        <v>1030</v>
       </c>
       <c r="B383" s="1">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="C383">
         <v>1</v>
@@ -25802,43 +25796,43 @@
     </row>
     <row r="384" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A384">
-        <v>1033</v>
+        <v>1030</v>
       </c>
       <c r="B384" s="1">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="C384">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="385" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A385">
-        <v>1033</v>
+        <v>1031</v>
       </c>
       <c r="B385" s="1">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="C385">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="386" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A386">
-        <v>1033</v>
+        <v>1031</v>
       </c>
       <c r="B386" s="1">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="C386">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="387" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A387">
-        <v>1034</v>
+        <v>1032</v>
       </c>
       <c r="B387" s="1">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="C387">
         <v>1</v>
@@ -25846,35 +25840,35 @@
     </row>
     <row r="388" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A388">
-        <v>1034</v>
+        <v>1033</v>
       </c>
       <c r="B388" s="1">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="C388">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="389" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A389">
-        <v>1034</v>
+        <v>1033</v>
       </c>
       <c r="B389" s="1">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="C389">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="390" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A390">
-        <v>1034</v>
+        <v>1033</v>
       </c>
       <c r="B390" s="1">
-        <v>382</v>
+        <v>378</v>
       </c>
       <c r="C390">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="391" spans="1:3" x14ac:dyDescent="0.2">
@@ -25882,10 +25876,10 @@
         <v>1034</v>
       </c>
       <c r="B391" s="1">
-        <v>383</v>
+        <v>379</v>
       </c>
       <c r="C391">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="392" spans="1:3" x14ac:dyDescent="0.2">
@@ -25893,9 +25887,53 @@
         <v>1034</v>
       </c>
       <c r="B392" s="1">
+        <v>380</v>
+      </c>
+      <c r="C392">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="393" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A393">
+        <v>1034</v>
+      </c>
+      <c r="B393" s="1">
+        <v>381</v>
+      </c>
+      <c r="C393">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="394" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A394">
+        <v>1034</v>
+      </c>
+      <c r="B394" s="1">
+        <v>382</v>
+      </c>
+      <c r="C394">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="395" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A395">
+        <v>1034</v>
+      </c>
+      <c r="B395" s="1">
+        <v>383</v>
+      </c>
+      <c r="C395">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="396" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A396">
+        <v>1034</v>
+      </c>
+      <c r="B396" s="1">
         <v>384</v>
       </c>
-      <c r="C392">
+      <c r="C396">
         <v>6</v>
       </c>
     </row>
@@ -25908,8 +25946,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I35"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="F35" sqref="F35"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -25970,7 +26008,7 @@
       <c r="E2" t="s">
         <v>389</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="9" t="s">
         <v>172</v>
       </c>
       <c r="G2" s="4" t="s">
@@ -25996,7 +26034,7 @@
       <c r="E3" s="7" t="s">
         <v>389</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="9" t="s">
         <v>172</v>
       </c>
       <c r="G3" s="7" t="s">
@@ -26022,14 +26060,14 @@
       <c r="E4" t="s">
         <v>389</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="9" t="s">
         <v>172</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>11</v>
       </c>
       <c r="H4" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
@@ -26048,7 +26086,7 @@
       <c r="E5" t="s">
         <v>389</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="9" t="s">
         <v>172</v>
       </c>
       <c r="G5" s="4" t="s">
@@ -26074,7 +26112,7 @@
       <c r="E6" t="s">
         <v>389</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="9" t="s">
         <v>172</v>
       </c>
       <c r="G6" s="4" t="s">
@@ -26100,7 +26138,7 @@
       <c r="E7" t="s">
         <v>389</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7" s="9" t="s">
         <v>172</v>
       </c>
       <c r="G7" t="s">
@@ -26129,7 +26167,7 @@
       <c r="E8" t="s">
         <v>389</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8" s="9" t="s">
         <v>172</v>
       </c>
       <c r="G8" t="s">
@@ -26158,7 +26196,7 @@
       <c r="E9" t="s">
         <v>389</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F9" s="9" t="s">
         <v>172</v>
       </c>
       <c r="G9" t="s">
@@ -26187,7 +26225,7 @@
       <c r="E10" t="s">
         <v>390</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F10" s="9" t="s">
         <v>172</v>
       </c>
       <c r="G10" s="4" t="s">
@@ -26213,7 +26251,7 @@
       <c r="E11" t="s">
         <v>390</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F11" s="9" t="s">
         <v>172</v>
       </c>
       <c r="G11" t="s">
@@ -26239,7 +26277,7 @@
       <c r="E12" t="s">
         <v>390</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F12" s="9" t="s">
         <v>172</v>
       </c>
       <c r="G12" s="4" t="s">
@@ -26265,7 +26303,7 @@
       <c r="E13" t="s">
         <v>390</v>
       </c>
-      <c r="F13" t="s">
+      <c r="F13" s="9" t="s">
         <v>172</v>
       </c>
       <c r="G13" s="4" t="s">
@@ -26291,7 +26329,7 @@
       <c r="E14" t="s">
         <v>390</v>
       </c>
-      <c r="F14" t="s">
+      <c r="F14" s="9" t="s">
         <v>172</v>
       </c>
       <c r="G14" s="4" t="s">
@@ -26317,14 +26355,14 @@
       <c r="E15" s="8" t="s">
         <v>390</v>
       </c>
-      <c r="F15" t="s">
+      <c r="F15" s="9" t="s">
         <v>172</v>
       </c>
       <c r="G15" s="8" t="s">
         <v>11</v>
       </c>
       <c r="H15" s="8" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="I15" s="8"/>
     </row>
@@ -26344,14 +26382,14 @@
       <c r="E16" s="8" t="s">
         <v>390</v>
       </c>
-      <c r="F16" t="s">
+      <c r="F16" s="9" t="s">
         <v>172</v>
       </c>
       <c r="G16" s="8" t="s">
         <v>29</v>
       </c>
       <c r="H16" s="8" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="I16" s="8" t="s">
         <v>302</v>
@@ -26373,7 +26411,7 @@
       <c r="E17" s="8" t="s">
         <v>390</v>
       </c>
-      <c r="F17" t="s">
+      <c r="F17" s="9" t="s">
         <v>172</v>
       </c>
       <c r="G17" s="8" t="s">
@@ -26402,7 +26440,7 @@
       <c r="E18" t="s">
         <v>390</v>
       </c>
-      <c r="F18" t="s">
+      <c r="F18" s="9" t="s">
         <v>172</v>
       </c>
       <c r="G18" t="s">
@@ -26431,7 +26469,7 @@
       <c r="E19" t="s">
         <v>390</v>
       </c>
-      <c r="F19" t="s">
+      <c r="F19" s="9" t="s">
         <v>172</v>
       </c>
       <c r="G19" t="s">
@@ -26460,7 +26498,7 @@
       <c r="E20" t="s">
         <v>390</v>
       </c>
-      <c r="F20" t="s">
+      <c r="F20" s="9" t="s">
         <v>172</v>
       </c>
       <c r="G20" t="s">
@@ -26486,7 +26524,7 @@
       <c r="E21" t="s">
         <v>390</v>
       </c>
-      <c r="F21" t="s">
+      <c r="F21" s="9" t="s">
         <v>172</v>
       </c>
       <c r="G21" s="4" t="s">
@@ -26512,7 +26550,7 @@
       <c r="E22" t="s">
         <v>390</v>
       </c>
-      <c r="F22" t="s">
+      <c r="F22" s="9" t="s">
         <v>172</v>
       </c>
       <c r="G22" s="4" t="s">
@@ -26538,7 +26576,7 @@
       <c r="E23" t="s">
         <v>390</v>
       </c>
-      <c r="F23" t="s">
+      <c r="F23" s="9" t="s">
         <v>172</v>
       </c>
       <c r="G23" s="4" t="s">
@@ -26564,7 +26602,7 @@
       <c r="E24" t="s">
         <v>390</v>
       </c>
-      <c r="F24" t="s">
+      <c r="F24" s="9" t="s">
         <v>172</v>
       </c>
       <c r="G24" s="4" t="s">
@@ -26590,7 +26628,7 @@
       <c r="E25" t="s">
         <v>390</v>
       </c>
-      <c r="F25" t="s">
+      <c r="F25" s="9" t="s">
         <v>172</v>
       </c>
       <c r="G25" s="7" t="s">
@@ -26619,7 +26657,7 @@
       <c r="E26" t="s">
         <v>390</v>
       </c>
-      <c r="F26" t="s">
+      <c r="F26" s="9" t="s">
         <v>172</v>
       </c>
       <c r="G26" s="7" t="s">
@@ -26648,7 +26686,7 @@
       <c r="E27" t="s">
         <v>390</v>
       </c>
-      <c r="F27" t="s">
+      <c r="F27" s="9" t="s">
         <v>172</v>
       </c>
       <c r="G27" s="7" t="s">
@@ -26677,7 +26715,7 @@
       <c r="E28" t="s">
         <v>390</v>
       </c>
-      <c r="F28" t="s">
+      <c r="F28" s="9" t="s">
         <v>172</v>
       </c>
       <c r="G28" s="7" t="s">
@@ -26703,7 +26741,7 @@
       <c r="E29" t="s">
         <v>390</v>
       </c>
-      <c r="F29" t="s">
+      <c r="F29" s="9" t="s">
         <v>172</v>
       </c>
       <c r="G29" s="4" t="s">
@@ -26729,7 +26767,7 @@
       <c r="E30" t="s">
         <v>390</v>
       </c>
-      <c r="F30" t="s">
+      <c r="F30" s="9" t="s">
         <v>172</v>
       </c>
       <c r="G30" s="4" t="s">
@@ -26755,7 +26793,7 @@
       <c r="E31" t="s">
         <v>390</v>
       </c>
-      <c r="F31" t="s">
+      <c r="F31" s="9" t="s">
         <v>172</v>
       </c>
       <c r="G31" s="4" t="s">
@@ -26781,7 +26819,7 @@
       <c r="E32" t="s">
         <v>390</v>
       </c>
-      <c r="F32" t="s">
+      <c r="F32" s="9" t="s">
         <v>172</v>
       </c>
       <c r="G32" s="7" t="s">
@@ -26810,7 +26848,7 @@
       <c r="E33" t="s">
         <v>390</v>
       </c>
-      <c r="F33" t="s">
+      <c r="F33" s="9" t="s">
         <v>172</v>
       </c>
       <c r="G33" s="7" t="s">
@@ -26839,7 +26877,7 @@
       <c r="E34" t="s">
         <v>390</v>
       </c>
-      <c r="F34" t="s">
+      <c r="F34" s="9" t="s">
         <v>172</v>
       </c>
       <c r="G34" s="7" t="s">
@@ -26868,7 +26906,7 @@
       <c r="E35" t="s">
         <v>390</v>
       </c>
-      <c r="F35" t="s">
+      <c r="F35" s="9" t="s">
         <v>172</v>
       </c>
       <c r="G35" s="7" t="s">
@@ -27470,8 +27508,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I61"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="D55" sqref="D55"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -27532,14 +27570,14 @@
       <c r="E2" t="s">
         <v>391</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="1" t="s">
         <v>172</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>7</v>
       </c>
       <c r="H2" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
@@ -27558,14 +27596,14 @@
       <c r="E3" t="s">
         <v>391</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="1" t="s">
         <v>172</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>11</v>
       </c>
       <c r="H3" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
@@ -27584,7 +27622,7 @@
       <c r="E4" t="s">
         <v>391</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="1" t="s">
         <v>172</v>
       </c>
       <c r="G4" t="s">
@@ -27613,7 +27651,7 @@
       <c r="E5" t="s">
         <v>391</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="1" t="s">
         <v>172</v>
       </c>
       <c r="G5" t="s">
@@ -27642,7 +27680,7 @@
       <c r="E6" t="s">
         <v>391</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="1" t="s">
         <v>172</v>
       </c>
       <c r="G6" t="s">
@@ -27671,7 +27709,7 @@
       <c r="E7" t="s">
         <v>391</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7" s="1" t="s">
         <v>172</v>
       </c>
       <c r="G7" t="s">
@@ -27700,14 +27738,14 @@
       <c r="E8" t="s">
         <v>391</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8" s="1" t="s">
         <v>172</v>
       </c>
       <c r="G8" t="s">
         <v>29</v>
       </c>
       <c r="H8" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="I8" t="s">
         <v>192</v>
@@ -27729,14 +27767,14 @@
       <c r="E9" t="s">
         <v>391</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F9" s="1" t="s">
         <v>172</v>
       </c>
       <c r="G9" t="s">
         <v>29</v>
       </c>
       <c r="H9" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="I9" t="s">
         <v>191</v>
@@ -27758,14 +27796,14 @@
       <c r="E10" t="s">
         <v>391</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F10" s="1" t="s">
         <v>172</v>
       </c>
       <c r="G10" t="s">
         <v>29</v>
       </c>
       <c r="H10" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="I10" t="s">
         <v>191</v>
@@ -27787,14 +27825,14 @@
       <c r="E11" t="s">
         <v>391</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F11" s="1" t="s">
         <v>172</v>
       </c>
       <c r="G11" t="s">
         <v>29</v>
       </c>
       <c r="H11" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="I11" t="s">
         <v>325</v>
@@ -27816,14 +27854,14 @@
       <c r="E12" t="s">
         <v>391</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F12" s="1" t="s">
         <v>172</v>
       </c>
       <c r="G12" s="4" t="s">
         <v>11</v>
       </c>
       <c r="H12" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
@@ -27842,14 +27880,14 @@
       <c r="E13" t="s">
         <v>391</v>
       </c>
-      <c r="F13" t="s">
+      <c r="F13" s="1" t="s">
         <v>172</v>
       </c>
       <c r="G13" s="4" t="s">
         <v>11</v>
       </c>
       <c r="H13" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
@@ -27868,7 +27906,7 @@
       <c r="E14" t="s">
         <v>391</v>
       </c>
-      <c r="F14" t="s">
+      <c r="F14" s="1" t="s">
         <v>172</v>
       </c>
       <c r="G14" t="s">
@@ -27897,7 +27935,7 @@
       <c r="E15" t="s">
         <v>391</v>
       </c>
-      <c r="F15" t="s">
+      <c r="F15" s="1" t="s">
         <v>172</v>
       </c>
       <c r="G15" t="s">
@@ -27926,7 +27964,7 @@
       <c r="E16" t="s">
         <v>391</v>
       </c>
-      <c r="F16" t="s">
+      <c r="F16" s="1" t="s">
         <v>172</v>
       </c>
       <c r="G16" t="s">
@@ -27955,7 +27993,7 @@
       <c r="E17" t="s">
         <v>391</v>
       </c>
-      <c r="F17" t="s">
+      <c r="F17" s="1" t="s">
         <v>172</v>
       </c>
       <c r="G17" t="s">
@@ -27984,14 +28022,14 @@
       <c r="E18" t="s">
         <v>392</v>
       </c>
-      <c r="F18" t="s">
+      <c r="F18" s="1" t="s">
         <v>172</v>
       </c>
       <c r="G18" s="4" t="s">
         <v>7</v>
       </c>
       <c r="H18" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
@@ -28010,14 +28048,14 @@
       <c r="E19" t="s">
         <v>392</v>
       </c>
-      <c r="F19" t="s">
+      <c r="F19" s="1" t="s">
         <v>172</v>
       </c>
       <c r="G19" t="s">
         <v>35</v>
       </c>
       <c r="H19" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
@@ -28025,10 +28063,10 @@
         <v>718</v>
       </c>
       <c r="B20">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="C20">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D20">
         <v>245</v>
@@ -28036,7 +28074,7 @@
       <c r="E20" t="s">
         <v>392</v>
       </c>
-      <c r="F20" t="s">
+      <c r="F20" s="1" t="s">
         <v>172</v>
       </c>
       <c r="G20" s="4" t="s">
@@ -28062,7 +28100,7 @@
       <c r="E21" t="s">
         <v>392</v>
       </c>
-      <c r="F21" t="s">
+      <c r="F21" s="1" t="s">
         <v>172</v>
       </c>
       <c r="G21" t="s">
@@ -28091,7 +28129,7 @@
       <c r="E22" t="s">
         <v>392</v>
       </c>
-      <c r="F22" t="s">
+      <c r="F22" s="1" t="s">
         <v>172</v>
       </c>
       <c r="G22" t="s">
@@ -28120,7 +28158,7 @@
       <c r="E23" t="s">
         <v>392</v>
       </c>
-      <c r="F23" t="s">
+      <c r="F23" s="1" t="s">
         <v>172</v>
       </c>
       <c r="G23" t="s">
@@ -28149,7 +28187,7 @@
       <c r="E24" t="s">
         <v>392</v>
       </c>
-      <c r="F24" t="s">
+      <c r="F24" s="1" t="s">
         <v>172</v>
       </c>
       <c r="G24" s="4" t="s">
@@ -28167,7 +28205,7 @@
         <v>716</v>
       </c>
       <c r="C25">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D25">
         <v>245</v>
@@ -28175,14 +28213,14 @@
       <c r="E25" t="s">
         <v>392</v>
       </c>
-      <c r="F25" t="s">
+      <c r="F25" s="1" t="s">
         <v>172</v>
       </c>
       <c r="G25" s="4" t="s">
         <v>11</v>
       </c>
       <c r="H25" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
@@ -28201,7 +28239,7 @@
       <c r="E26" t="s">
         <v>392</v>
       </c>
-      <c r="F26" t="s">
+      <c r="F26" s="1" t="s">
         <v>172</v>
       </c>
       <c r="G26" t="s">
@@ -28230,7 +28268,7 @@
       <c r="E27" t="s">
         <v>392</v>
       </c>
-      <c r="F27" t="s">
+      <c r="F27" s="1" t="s">
         <v>172</v>
       </c>
       <c r="G27" t="s">
@@ -28251,7 +28289,7 @@
         <v>716</v>
       </c>
       <c r="C28">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D28">
         <v>245</v>
@@ -28259,14 +28297,14 @@
       <c r="E28" t="s">
         <v>392</v>
       </c>
-      <c r="F28" t="s">
+      <c r="F28" s="1" t="s">
         <v>172</v>
       </c>
       <c r="G28" t="s">
         <v>35</v>
       </c>
       <c r="H28" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
@@ -28285,7 +28323,7 @@
       <c r="E29" t="s">
         <v>392</v>
       </c>
-      <c r="F29" t="s">
+      <c r="F29" s="1" t="s">
         <v>172</v>
       </c>
       <c r="G29" t="s">
@@ -28314,7 +28352,7 @@
       <c r="E30" t="s">
         <v>392</v>
       </c>
-      <c r="F30" t="s">
+      <c r="F30" s="1" t="s">
         <v>172</v>
       </c>
       <c r="G30" t="s">
@@ -28343,7 +28381,7 @@
       <c r="E31" t="s">
         <v>393</v>
       </c>
-      <c r="F31" t="s">
+      <c r="F31" s="1" t="s">
         <v>172</v>
       </c>
       <c r="G31" s="4" t="s">
@@ -28369,7 +28407,7 @@
       <c r="E32" t="s">
         <v>393</v>
       </c>
-      <c r="F32" t="s">
+      <c r="F32" s="1" t="s">
         <v>172</v>
       </c>
       <c r="G32" s="4" t="s">
@@ -28395,7 +28433,7 @@
       <c r="E33" t="s">
         <v>393</v>
       </c>
-      <c r="F33" t="s">
+      <c r="F33" s="1" t="s">
         <v>172</v>
       </c>
       <c r="G33" t="s">
@@ -28424,7 +28462,7 @@
       <c r="E34" t="s">
         <v>393</v>
       </c>
-      <c r="F34" t="s">
+      <c r="F34" s="1" t="s">
         <v>172</v>
       </c>
       <c r="G34" t="s">
@@ -28453,7 +28491,7 @@
       <c r="E35" t="s">
         <v>393</v>
       </c>
-      <c r="F35" t="s">
+      <c r="F35" s="1" t="s">
         <v>172</v>
       </c>
       <c r="G35" s="4" t="s">
@@ -28479,7 +28517,7 @@
       <c r="E36" t="s">
         <v>393</v>
       </c>
-      <c r="F36" t="s">
+      <c r="F36" s="1" t="s">
         <v>172</v>
       </c>
       <c r="G36" s="7" t="s">
@@ -28508,7 +28546,7 @@
       <c r="E37" t="s">
         <v>394</v>
       </c>
-      <c r="F37" t="s">
+      <c r="F37" s="1" t="s">
         <v>172</v>
       </c>
       <c r="G37" s="4" t="s">
@@ -28534,7 +28572,7 @@
       <c r="E38" t="s">
         <v>394</v>
       </c>
-      <c r="F38" t="s">
+      <c r="F38" s="1" t="s">
         <v>172</v>
       </c>
       <c r="G38" s="4" t="s">
@@ -28560,7 +28598,7 @@
       <c r="E39" t="s">
         <v>394</v>
       </c>
-      <c r="F39" t="s">
+      <c r="F39" s="1" t="s">
         <v>172</v>
       </c>
       <c r="G39" t="s">
@@ -28586,7 +28624,7 @@
       <c r="E40" t="s">
         <v>394</v>
       </c>
-      <c r="F40" t="s">
+      <c r="F40" s="1" t="s">
         <v>172</v>
       </c>
       <c r="G40" s="7" t="s">
@@ -28615,7 +28653,7 @@
       <c r="E41" t="s">
         <v>394</v>
       </c>
-      <c r="F41" t="s">
+      <c r="F41" s="1" t="s">
         <v>172</v>
       </c>
       <c r="G41" s="7" t="s">
@@ -28644,7 +28682,7 @@
       <c r="E42" t="s">
         <v>394</v>
       </c>
-      <c r="F42" t="s">
+      <c r="F42" s="1" t="s">
         <v>172</v>
       </c>
       <c r="G42" s="7" t="s">
@@ -28662,10 +28700,10 @@
         <v>741</v>
       </c>
       <c r="B43">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="C43">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D43">
         <v>254</v>
@@ -28673,7 +28711,7 @@
       <c r="E43" t="s">
         <v>394</v>
       </c>
-      <c r="F43" t="s">
+      <c r="F43" s="1" t="s">
         <v>172</v>
       </c>
       <c r="G43" s="7" t="s">
@@ -28699,7 +28737,7 @@
       <c r="E44" t="s">
         <v>394</v>
       </c>
-      <c r="F44" t="s">
+      <c r="F44" s="1" t="s">
         <v>172</v>
       </c>
       <c r="G44" s="7" t="s">
@@ -28728,7 +28766,7 @@
       <c r="E45" t="s">
         <v>394</v>
       </c>
-      <c r="F45" t="s">
+      <c r="F45" s="1" t="s">
         <v>172</v>
       </c>
       <c r="G45" s="7" t="s">
@@ -28746,10 +28784,10 @@
         <v>744</v>
       </c>
       <c r="B46">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="C46">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D46">
         <v>254</v>
@@ -28757,7 +28795,7 @@
       <c r="E46" t="s">
         <v>394</v>
       </c>
-      <c r="F46" t="s">
+      <c r="F46" s="1" t="s">
         <v>172</v>
       </c>
       <c r="G46" s="7" t="s">
@@ -28775,10 +28813,10 @@
         <v>745</v>
       </c>
       <c r="B47">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="C47">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D47">
         <v>254</v>
@@ -28786,7 +28824,7 @@
       <c r="E47" t="s">
         <v>394</v>
       </c>
-      <c r="F47" t="s">
+      <c r="F47" s="1" t="s">
         <v>172</v>
       </c>
       <c r="G47" s="7" t="s">
@@ -28812,7 +28850,7 @@
       <c r="E48" t="s">
         <v>394</v>
       </c>
-      <c r="F48" t="s">
+      <c r="F48" s="1" t="s">
         <v>172</v>
       </c>
       <c r="G48" s="7" t="s">
@@ -28841,7 +28879,7 @@
       <c r="E49" t="s">
         <v>394</v>
       </c>
-      <c r="F49" t="s">
+      <c r="F49" s="1" t="s">
         <v>172</v>
       </c>
       <c r="G49" s="7" t="s">
@@ -28859,10 +28897,10 @@
         <v>748</v>
       </c>
       <c r="B50">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="C50">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D50">
         <v>254</v>
@@ -28870,7 +28908,7 @@
       <c r="E50" t="s">
         <v>394</v>
       </c>
-      <c r="F50" t="s">
+      <c r="F50" s="1" t="s">
         <v>172</v>
       </c>
       <c r="G50" s="4" t="s">
@@ -28888,7 +28926,7 @@
         <v>736</v>
       </c>
       <c r="C51">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D51">
         <v>255</v>
@@ -28896,7 +28934,7 @@
       <c r="E51" t="s">
         <v>394</v>
       </c>
-      <c r="F51" t="s">
+      <c r="F51" s="1" t="s">
         <v>172</v>
       </c>
       <c r="G51" s="4" t="s">
@@ -28922,7 +28960,7 @@
       <c r="E52" t="s">
         <v>394</v>
       </c>
-      <c r="F52" t="s">
+      <c r="F52" s="1" t="s">
         <v>172</v>
       </c>
       <c r="G52" s="7" t="s">
@@ -28951,7 +28989,7 @@
       <c r="E53" t="s">
         <v>394</v>
       </c>
-      <c r="F53" t="s">
+      <c r="F53" s="1" t="s">
         <v>172</v>
       </c>
       <c r="G53" s="7" t="s">
@@ -28980,7 +29018,7 @@
       <c r="E54" t="s">
         <v>394</v>
       </c>
-      <c r="F54" t="s">
+      <c r="F54" s="1" t="s">
         <v>172</v>
       </c>
       <c r="G54" s="7" t="s">
@@ -29009,7 +29047,7 @@
       <c r="E55" t="s">
         <v>394</v>
       </c>
-      <c r="F55" t="s">
+      <c r="F55" s="1" t="s">
         <v>172</v>
       </c>
       <c r="G55" s="7" t="s">
@@ -29038,7 +29076,7 @@
       <c r="E56" t="s">
         <v>394</v>
       </c>
-      <c r="F56" t="s">
+      <c r="F56" s="1" t="s">
         <v>172</v>
       </c>
       <c r="G56" s="7" t="s">
@@ -29067,7 +29105,7 @@
       <c r="E57" t="s">
         <v>394</v>
       </c>
-      <c r="F57" t="s">
+      <c r="F57" s="1" t="s">
         <v>172</v>
       </c>
       <c r="G57" s="7" t="s">
@@ -29096,14 +29134,14 @@
       <c r="E58" s="8" t="s">
         <v>394</v>
       </c>
-      <c r="F58" t="s">
+      <c r="F58" s="1" t="s">
         <v>172</v>
       </c>
       <c r="G58" s="8" t="s">
         <v>6</v>
       </c>
       <c r="H58" s="8" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="I58" s="8"/>
     </row>
@@ -29123,7 +29161,7 @@
       <c r="E59" t="s">
         <v>394</v>
       </c>
-      <c r="F59" t="s">
+      <c r="F59" s="1" t="s">
         <v>172</v>
       </c>
       <c r="G59" s="7" t="s">
@@ -29152,7 +29190,7 @@
       <c r="E60" t="s">
         <v>394</v>
       </c>
-      <c r="F60" t="s">
+      <c r="F60" s="1" t="s">
         <v>172</v>
       </c>
       <c r="G60" s="7" t="s">
@@ -29181,7 +29219,7 @@
       <c r="E61" t="s">
         <v>394</v>
       </c>
-      <c r="F61" t="s">
+      <c r="F61" s="1" t="s">
         <v>172</v>
       </c>
       <c r="G61" s="7" t="s">
@@ -29196,6 +29234,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -29204,7 +29243,7 @@
   <dimension ref="A1:C49"/>
   <sheetViews>
     <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B50" sqref="B50"/>
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>

</xml_diff>